<commit_message>
Add previousVersion metadata, update 1.0.0
</commit_message>
<xml_diff>
--- a/controlled-vocabulary-template/controlled-vocabulary-template.xlsx
+++ b/controlled-vocabulary-template/controlled-vocabulary-template.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabulary-template\my-vocabulary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabulary-template\controlled-vocabulary-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CFEFF3-FE7B-419A-8E47-EB9211572888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20F6791-F61B-4A53-8644-03B6781C5F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Controlled Vocabulary" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>dct:title</t>
   </si>
@@ -154,28 +152,31 @@
     <t>Publisher</t>
   </si>
   <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>Name Surname (Affiliation)</t>
+  </si>
+  <si>
+    <t>OtherName OtherSurname (OtherAffiliation)</t>
+  </si>
+  <si>
+    <t>My comments (not parsed by the tool).</t>
+  </si>
+  <si>
+    <t>Template Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>Template for generating a controlled vocabulary defined under a certain my-namespace.</t>
+  </si>
+  <si>
+    <t>https://w3id.org/my-namespace/controlled-vocabulary-template</t>
+  </si>
+  <si>
+    <t>owl:priorVersion</t>
+  </si>
+  <si>
     <t>1.0.0</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/licenses/by/4.0/</t>
-  </si>
-  <si>
-    <t>Name Surname (Affiliation)</t>
-  </si>
-  <si>
-    <t>OtherName OtherSurname (OtherAffiliation)</t>
-  </si>
-  <si>
-    <t>My comments (not parsed by the tool).</t>
-  </si>
-  <si>
-    <t>Template Controlled Vocabulary</t>
-  </si>
-  <si>
-    <t>Template for generating a controlled vocabulary defined under a certain my-namespace.</t>
-  </si>
-  <si>
-    <t>https://w3id.org/my-namespace/controlled-vocabulary-template</t>
   </si>
 </sst>
 </file>
@@ -561,80 +562,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89.42578125" customWidth="1"/>
-    <col min="2" max="2" width="74.7109375" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -643,34 +632,34 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -680,250 +669,257 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B17)," ","-"))</f>
+    <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B18)," ","-"))</f>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-1</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f t="shared" ref="A18:A40" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B18)," ","-"))</f>
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" ref="A19:A41" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B19)," ","-"))</f>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-2</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
+    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-3</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
+    <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-4</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
+    <row r="22" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-5</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
+    <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-6</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
+    <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-7</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
+    <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-8</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
+    <row r="26" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-9</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
+    <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-10</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
+    <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-11</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
+    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-12</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
+    <row r="30" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-13</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
+    <row r="31" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-14</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
+    <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-15</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-16</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-17</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-16</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-18</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-17</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-19</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-18</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-20</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-19</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-21</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-20</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-22</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-21</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-23</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-22</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-23</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-24</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B41" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -931,21 +927,9 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{8D37ED2A-6F4C-4B2C-B212-84B5255111B4}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add bibo:status metadata, update 1.0.0
</commit_message>
<xml_diff>
--- a/controlled-vocabulary-template/controlled-vocabulary-template.xlsx
+++ b/controlled-vocabulary-template/controlled-vocabulary-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabulary-template\controlled-vocabulary-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20F6791-F61B-4A53-8644-03B6781C5F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC39D08-CE1F-4E36-92AA-234FBBD125EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlled Vocabulary" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>dct:title</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>1.0.0</t>
+  </si>
+  <si>
+    <t>http://purl.org/ontology/bibo/status</t>
+  </si>
+  <si>
+    <t>Draft Controlled Vocabulary</t>
   </si>
 </sst>
 </file>
@@ -563,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,241 +691,249 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B18)," ","-"))</f>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-1</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" ref="A19:A41" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B19)," ","-"))</f>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-2</v>
+        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B19)," ","-"))</f>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-1</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-3</v>
+        <f t="shared" ref="A20:A42" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(LOWER(B20)," ","-"))</f>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-2</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-4</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-3</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-5</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-4</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-6</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-5</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-7</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-6</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-8</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-7</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-9</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-8</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-10</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-9</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-11</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-10</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-12</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-11</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-13</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-12</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-14</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-13</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-15</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-14</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-16</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-15</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-17</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-16</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-18</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-17</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-19</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-18</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-20</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-19</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-21</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-20</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-22</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-21</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
-        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-23</v>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-22</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
+        <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-23</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f t="shared" si="0"/>
         <v>https://w3id.org/my-namespace/controlled-vocabulary-template/my-term-24</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B42" s="7" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>